<commit_message>
dvdasa stats updated again, people like critter
</commit_message>
<xml_diff>
--- a/dvdasa visit numbers.xlsx
+++ b/dvdasa visit numbers.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Link</t>
   </si>
@@ -189,6 +184,24 @@
   </si>
   <si>
     <t>http://www.dvdasa.com/index.php?title=Saga_02_:_Chapter_002_:_Sardines</t>
+  </si>
+  <si>
+    <t>10/17 at 1AM</t>
+  </si>
+  <si>
+    <t>http://dvdasa.com/index.php?title=File:THREATLEVEL_VITAMINPISSYELLOW.jpg</t>
+  </si>
+  <si>
+    <t>http://dvdasa.com/index.php?title=File:Joe_rogan_flick.jpg</t>
+  </si>
+  <si>
+    <t>http://dvdasa.com/index.php?title=CRITTER%27S_CROSS_COUNTRY_CASH_CONTEST</t>
+  </si>
+  <si>
+    <t>http://dvdasa.com/index.php?title=Joe_Rogan</t>
+  </si>
+  <si>
+    <t>http://dvdasa.com/index.php?title=Glossary</t>
   </si>
 </sst>
 </file>
@@ -506,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,11 +527,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -526,15 +539,16 @@
     <col min="1" max="1" width="81.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,8 +558,11 @@
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -555,8 +572,11 @@
       <c r="C3" s="1">
         <v>22130</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>32944</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,544 +586,764 @@
       <c r="C4" s="1">
         <v>3025</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>4085</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7902</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
         <v>129</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B9" s="1">
         <v>677</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C9" s="1">
         <v>976</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="D9" s="1">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B10" s="1">
         <v>785</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C10" s="1">
         <v>1134</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="D10" s="1">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B11" s="1">
         <v>475</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C11" s="1">
         <v>640</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="D11" s="1">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B12" s="1">
         <v>309</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C12" s="1">
         <v>434</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="D12" s="1">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B13" s="1">
         <v>301</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C13" s="1">
         <v>403</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="D13" s="1">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B14" s="1">
         <v>318</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C14" s="1">
         <v>422</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="D14" s="1">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B15" s="1">
         <v>316</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C15" s="1">
         <v>418</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="D15" s="1">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B16" s="1">
         <v>226</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C16" s="1">
         <v>325</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="D16" s="1">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B17" s="1">
         <v>187</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C17" s="1">
         <v>285</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="D17" s="1">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B18" s="1">
         <v>209</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C18" s="1">
         <v>317</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="D18" s="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B19" s="1">
         <v>350</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C19" s="1">
         <v>496</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="D19" s="1">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B20" s="1">
         <v>236</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C20" s="1">
         <v>340</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="D20" s="1">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B21" s="1">
         <v>290</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C21" s="1">
         <v>431</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="D21" s="1">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B22" s="1">
         <v>149</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C22" s="1">
         <v>222</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="D22" s="1">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B23" s="1">
         <v>214</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C23" s="1">
         <v>282</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="D23" s="1">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B24" s="1">
         <v>286</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C24" s="1">
         <v>384</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="D24" s="1">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B27" s="1">
         <v>327</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C27" s="1">
         <v>404</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="D27" s="1">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B28" s="1">
         <v>228</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C28" s="1">
         <v>283</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="D28" s="1">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B29" s="1">
         <v>45</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C29" s="1">
         <v>92</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="D29" s="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B30" s="1">
         <v>53</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C30" s="1">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="D30" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B32" s="1">
         <v>236</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C32" s="1">
         <v>317</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="D32" s="1">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B34" s="1">
         <v>176</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C34" s="1">
         <v>266</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="D34" s="1">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B35" s="1">
         <v>195</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C35" s="1">
         <v>252</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="D35" s="1">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B36" s="1">
         <v>144</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C36" s="1">
         <v>203</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="D36" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B37" s="1">
         <v>116</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C37" s="1">
         <v>195</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="D37" s="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B38" s="1">
         <v>231</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C38" s="1">
         <v>310</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="D38" s="1">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B39" s="1">
         <v>500</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C39" s="1">
         <v>639</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="D39" s="1">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B40" s="1">
         <v>295</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C40" s="1">
         <v>387</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="D40" s="1">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B41" s="1">
         <v>271</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C41" s="1">
         <v>346</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="D41" s="1">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="1">
-        <v>0</v>
-      </c>
-      <c r="C38" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B43" s="1">
         <v>328</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C43" s="1">
         <v>431</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="D43" s="1">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B44" s="1">
         <v>201</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C44" s="1">
         <v>263</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="D44" s="1">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B45" s="1">
         <v>106</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C45" s="1">
         <v>154</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="D45" s="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="1">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1">
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="D46" s="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="1">
-        <v>0</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="1">
-        <v>0</v>
-      </c>
-      <c r="C44" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B49" s="1">
         <v>157</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C49" s="1">
         <v>239</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="D49" s="1">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B50" s="1">
         <v>170</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C50" s="1">
         <v>235</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="D50" s="1">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B51" s="1">
         <v>173</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C51" s="1">
         <v>244</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="D51" s="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B52" s="1">
         <v>138</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C52" s="1">
         <v>184</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="D52" s="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B53" s="1">
         <v>251</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C53" s="1">
         <v>319</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="D53" s="1">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B54" s="1">
         <v>61</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C54" s="1">
         <v>82</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B55" s="1">
         <v>13</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C55" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="D55" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="1">
-        <v>0</v>
-      </c>
-      <c r="C52" s="1">
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="1">
-        <v>0</v>
-      </c>
-      <c r="C53" s="1">
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1">
         <v>23</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dvdasa visit #s saved and uploaded on 10.19 at 101
</commit_message>
<xml_diff>
--- a/dvdasa visit numbers.xlsx
+++ b/dvdasa visit numbers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t>Link</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Projects</t>
+  </si>
+  <si>
+    <t>10/19 at 12:45AM</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -496,8 +498,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="373468552"/>
-        <c:axId val="373458360"/>
+        <c:axId val="278305856"/>
+        <c:axId val="278299584"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -582,11 +584,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="376851808"/>
-        <c:axId val="376844360"/>
+        <c:axId val="278305072"/>
+        <c:axId val="278304680"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="373468552"/>
+        <c:axId val="278305856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,14 +631,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373458360"/>
+        <c:crossAx val="278299584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="373458360"/>
+        <c:axId val="278299584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,12 +689,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373468552"/>
+        <c:crossAx val="278305856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="376844360"/>
+        <c:axId val="278304680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -729,12 +731,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376851808"/>
+        <c:crossAx val="278305072"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="376851808"/>
+        <c:axId val="278305072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -744,7 +746,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="376844360"/>
+        <c:crossAx val="278304680"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -759,7 +762,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1683,30 +1685,31 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="21" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="19.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="21.5703125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="22.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1725,8 +1728,11 @@
       <c r="F2" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1745,8 +1751,11 @@
       <c r="F3" s="1">
         <v>46266</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>57344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1765,8 +1774,11 @@
       <c r="F4" s="1">
         <v>5928</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>7275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -1785,8 +1797,11 @@
       <c r="F5" s="1">
         <v>10501</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>12035</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -1805,8 +1820,11 @@
       <c r="F6" s="1">
         <v>3632</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
@@ -1816,8 +1834,11 @@
       <c r="F7" s="1">
         <v>345</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -1836,8 +1857,11 @@
       <c r="F8" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -1856,8 +1880,11 @@
       <c r="F9" s="1">
         <v>692</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1876,8 +1903,11 @@
       <c r="F10" s="1">
         <v>2520</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <v>3757</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1896,8 +1926,11 @@
       <c r="F11" s="1">
         <v>2820</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>3754</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1916,8 +1949,11 @@
       <c r="F12" s="1">
         <v>1528</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1936,8 +1972,11 @@
       <c r="F13" s="1">
         <v>1234</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1956,8 +1995,11 @@
       <c r="F14" s="1">
         <v>858</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1976,8 +2018,11 @@
       <c r="F15" s="1">
         <v>944</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1996,8 +2041,11 @@
       <c r="F16" s="1">
         <v>802</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2016,8 +2064,11 @@
       <c r="F17" s="1">
         <v>697</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -2036,8 +2087,11 @@
       <c r="F18" s="1">
         <v>618</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -2056,8 +2110,11 @@
       <c r="F19" s="1">
         <v>606</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -2076,8 +2133,11 @@
       <c r="F20" s="1">
         <v>1082</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -2096,8 +2156,11 @@
       <c r="F21" s="1">
         <v>805</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -2116,8 +2179,11 @@
       <c r="F22" s="1">
         <v>973</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -2136,8 +2202,11 @@
       <c r="F23" s="1">
         <v>449</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -2156,8 +2225,11 @@
       <c r="F24" s="1">
         <v>499</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -2176,8 +2248,11 @@
       <c r="F25" s="1">
         <v>1027</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="1">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -2196,8 +2271,11 @@
       <c r="F26" s="1">
         <v>187</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -2216,8 +2294,11 @@
       <c r="F27" s="1">
         <v>116</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2236,8 +2317,11 @@
       <c r="F28" s="1">
         <v>631</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -2256,8 +2340,11 @@
       <c r="F29" s="1">
         <v>560</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="1">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2276,8 +2363,11 @@
       <c r="F30" s="1">
         <v>226</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -2296,8 +2386,11 @@
       <c r="F31" s="1">
         <v>209</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>59</v>
       </c>
@@ -2316,8 +2409,11 @@
       <c r="F32" s="1">
         <v>758</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="1">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -2336,8 +2432,11 @@
       <c r="F33" s="1">
         <v>678</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="1">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
@@ -2356,8 +2455,11 @@
       <c r="F34" s="1">
         <v>664</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -2376,8 +2478,11 @@
       <c r="F35" s="1">
         <v>664</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="1">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
@@ -2396,8 +2501,11 @@
       <c r="F36" s="1">
         <v>414</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="1">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -2416,8 +2524,11 @@
       <c r="F37" s="1">
         <v>352</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="1">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -2427,8 +2538,11 @@
       <c r="F38" s="1">
         <v>114</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -2447,8 +2561,11 @@
       <c r="F39" s="1">
         <v>488</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="1">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
@@ -2458,8 +2575,11 @@
       <c r="F40" s="1">
         <v>111</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -2469,8 +2589,11 @@
       <c r="F41" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="1">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
@@ -2489,8 +2612,11 @@
       <c r="F42" s="1">
         <v>1320</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="1">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
@@ -2509,8 +2635,11 @@
       <c r="F43" s="1">
         <v>1347</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="1">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
@@ -2529,8 +2658,11 @@
       <c r="F44" s="1">
         <v>692</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="1">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
@@ -2549,8 +2681,11 @@
       <c r="F45" s="1">
         <v>686</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="1">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>37</v>
       </c>
@@ -2569,8 +2704,11 @@
       <c r="F46" s="1">
         <v>825</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>38</v>
       </c>
@@ -2589,8 +2727,11 @@
       <c r="F47" s="1">
         <v>402</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="1">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>39</v>
       </c>
@@ -2609,8 +2750,11 @@
       <c r="F48" s="1">
         <v>403</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="1">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>40</v>
       </c>
@@ -2629,8 +2773,11 @@
       <c r="F49" s="1">
         <v>334</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="1">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>41</v>
       </c>
@@ -2649,8 +2796,11 @@
       <c r="F50" s="1">
         <v>226</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="1">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
@@ -2669,8 +2819,11 @@
       <c r="F51" s="1">
         <v>221</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="1">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
@@ -2689,8 +2842,11 @@
       <c r="F52" s="1">
         <v>246</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="1">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>44</v>
       </c>
@@ -2709,8 +2865,11 @@
       <c r="F53" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="1">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>45</v>
       </c>
@@ -2729,8 +2888,11 @@
       <c r="F54" s="1">
         <v>429</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="1">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>46</v>
       </c>
@@ -2749,8 +2911,11 @@
       <c r="F55" s="1">
         <v>432</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="1">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>47</v>
       </c>
@@ -2769,8 +2934,11 @@
       <c r="F56" s="1">
         <v>302</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="1">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>48</v>
       </c>
@@ -2789,8 +2957,11 @@
       <c r="F57" s="1">
         <v>503</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="1">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>49</v>
       </c>
@@ -2809,8 +2980,11 @@
       <c r="F58" s="1">
         <v>135</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="1">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>50</v>
       </c>
@@ -2829,8 +3003,11 @@
       <c r="F59" s="1">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>52</v>
       </c>
@@ -2849,8 +3026,11 @@
       <c r="F60" s="1">
         <v>85</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>53</v>
       </c>
@@ -2869,8 +3049,11 @@
       <c r="F61" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>

</xml_diff>